<commit_message>
feat: search items by input in command line
</commit_message>
<xml_diff>
--- a/prices.xlsx
+++ b/prices.xlsx
@@ -67,7 +67,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -109,15 +109,15 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Официальный магазин LG</t>
+          <t>E-first.ru</t>
         </is>
       </c>
       <c r="C2" s="0" t="n">
-        <v>324.01</v>
+        <v>325.59</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>9 499 р.</t>
+          <t>9 535 р.</t>
         </is>
       </c>
     </row>
@@ -129,15 +129,15 @@
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>Goods.ru</t>
+          <t>Официальный магазин LG</t>
         </is>
       </c>
       <c r="C3" s="0" t="n">
-        <v>304.94</v>
+        <v>324.36</v>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>8 940 р.</t>
+          <t>9 499 р.</t>
         </is>
       </c>
     </row>
@@ -149,15 +149,15 @@
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Kns.ru</t>
+          <t>Goods.ru</t>
         </is>
       </c>
       <c r="C4" s="0" t="n">
-        <v>298.33</v>
+        <v>305.27</v>
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>8 746 р.</t>
+          <t>8 940 р.</t>
         </is>
       </c>
     </row>
@@ -169,15 +169,15 @@
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>Svyaznoy.ru</t>
+          <t>Kns.ru</t>
         </is>
       </c>
       <c r="C5" s="0" t="n">
-        <v>345.19</v>
+        <v>298.65</v>
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>10 120 р.</t>
+          <t>8 746 р.</t>
         </is>
       </c>
     </row>
@@ -189,15 +189,15 @@
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>Pleer.ru</t>
+          <t>Svyaznoy.ru</t>
         </is>
       </c>
       <c r="C6" s="0" t="n">
-        <v>275.95</v>
+        <v>345.56</v>
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>8 090 р.</t>
+          <t>10 120 р.</t>
         </is>
       </c>
     </row>
@@ -209,15 +209,15 @@
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>CompYou.ru</t>
+          <t>Pleer.ru</t>
         </is>
       </c>
       <c r="C7" s="0" t="n">
-        <v>297.95</v>
+        <v>286.12</v>
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>8 735 р.</t>
+          <t>8 379 р.</t>
         </is>
       </c>
     </row>
@@ -229,15 +229,15 @@
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>Eldorado.ru</t>
+          <t>CompYou.ru</t>
         </is>
       </c>
       <c r="C8" s="0" t="n">
-        <v>323.71</v>
+        <v>298.27</v>
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>9 490 р.</t>
+          <t>8 735 р.</t>
         </is>
       </c>
     </row>
@@ -249,15 +249,15 @@
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>Elektro-park.ru</t>
+          <t>Eldorado.ru</t>
         </is>
       </c>
       <c r="C9" s="0" t="n">
-        <v>305.63</v>
+        <v>324.05</v>
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>8 960 р.</t>
+          <t>9 490 р.</t>
         </is>
       </c>
     </row>
@@ -269,15 +269,15 @@
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>Citilink.ru</t>
+          <t>Elektro-park.ru</t>
         </is>
       </c>
       <c r="C10" s="0" t="n">
-        <v>306.65</v>
+        <v>305.95</v>
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>8 990 р.</t>
+          <t>8 960 р.</t>
         </is>
       </c>
     </row>
@@ -289,15 +289,15 @@
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>Fotosklad.ru</t>
+          <t>Citilink.ru</t>
         </is>
       </c>
       <c r="C11" s="0" t="n">
-        <v>316.88</v>
+        <v>306.98</v>
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>9 290 р.</t>
+          <t>8 990 р.</t>
         </is>
       </c>
     </row>
@@ -309,15 +309,15 @@
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>ABC.ru</t>
+          <t>Fotosklad.ru</t>
         </is>
       </c>
       <c r="C12" s="0" t="n">
-        <v>316.58</v>
+        <v>317.22</v>
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t>9 281 р.</t>
+          <t>9 290 р.</t>
         </is>
       </c>
     </row>
@@ -329,15 +329,15 @@
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>123.ru</t>
+          <t>ABC.ru</t>
         </is>
       </c>
       <c r="C13" s="0" t="n">
-        <v>312.11</v>
+        <v>316.92</v>
       </c>
       <c r="D13" s="0" t="inlineStr">
         <is>
-          <t>9 150 р.</t>
+          <t>9 281 р.</t>
         </is>
       </c>
     </row>
@@ -349,15 +349,15 @@
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>Technopoint.ru</t>
+          <t>123.ru</t>
         </is>
       </c>
       <c r="C14" s="0" t="n">
-        <v>306.96</v>
+        <v>312.44</v>
       </c>
       <c r="D14" s="0" t="inlineStr">
         <is>
-          <t>8 999 р.</t>
+          <t>9 150 р.</t>
         </is>
       </c>
     </row>
@@ -373,7 +373,7 @@
         </is>
       </c>
       <c r="C15" s="0" t="n">
-        <v>323.71</v>
+        <v>324.05</v>
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
@@ -393,7 +393,7 @@
         </is>
       </c>
       <c r="C16" s="0" t="n">
-        <v>310.06</v>
+        <v>310.39</v>
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
@@ -413,7 +413,7 @@
         </is>
       </c>
       <c r="C17" s="0" t="n">
-        <v>333.94</v>
+        <v>334.3</v>
       </c>
       <c r="D17" s="0" t="inlineStr">
         <is>
@@ -433,7 +433,7 @@
         </is>
       </c>
       <c r="C18" s="0" t="n">
-        <v>336.67</v>
+        <v>337.03</v>
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
@@ -453,11 +453,11 @@
         </is>
       </c>
       <c r="C19" s="0" t="n">
-        <v>285.84</v>
+        <v>285.81</v>
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
-          <t>8 380 р.</t>
+          <t>8 370 р.</t>
         </is>
       </c>
     </row>
@@ -469,11 +469,11 @@
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>Foroom.com.ua</t>
+          <t>Itbox.ua</t>
         </is>
       </c>
       <c r="C20" s="0" t="n">
-        <v>269.16</v>
+        <v>270.52</v>
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
@@ -489,11 +489,11 @@
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>A-techno.com.ua</t>
+          <t>LuxPRO.ua</t>
         </is>
       </c>
       <c r="C21" s="0" t="n">
-        <v>269.16</v>
+        <v>270.52</v>
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
@@ -509,15 +509,15 @@
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>Zhuk.ua</t>
+          <t>V10.com.ua</t>
         </is>
       </c>
       <c r="C22" s="0" t="n">
-        <v>269.16</v>
+        <v>393.02</v>
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t>2 999 грн.</t>
+          <t>4 357 грн.</t>
         </is>
       </c>
     </row>
@@ -529,15 +529,15 @@
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>Епіцентр</t>
+          <t>Foroom.com.ua</t>
         </is>
       </c>
       <c r="C23" s="0" t="n">
-        <v>269.16</v>
+        <v>306.97</v>
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t>2 999 грн.</t>
+          <t>3 403 грн.</t>
         </is>
       </c>
     </row>
@@ -549,15 +549,15 @@
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>АЛЛО</t>
+          <t>Repka.ua</t>
         </is>
       </c>
       <c r="C24" s="0" t="n">
-        <v>269.16</v>
+        <v>267.46</v>
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t>2 999 грн.</t>
+          <t>2 965 грн.</t>
         </is>
       </c>
     </row>
@@ -569,11 +569,11 @@
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>Denika.ua</t>
+          <t>A-techno.com.ua</t>
         </is>
       </c>
       <c r="C25" s="0" t="n">
-        <v>269.16</v>
+        <v>270.52</v>
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
@@ -589,15 +589,15 @@
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>Stylus.ua</t>
+          <t>Homebt.com.ua</t>
         </is>
       </c>
       <c r="C26" s="0" t="n">
-        <v>270.14</v>
+        <v>286.58</v>
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t>3 010 грн.</t>
+          <t>3 177 грн.</t>
         </is>
       </c>
     </row>
@@ -609,15 +609,15 @@
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>Цифра</t>
+          <t>Hbox.com.ua</t>
         </is>
       </c>
       <c r="C27" s="0" t="n">
-        <v>261.17</v>
+        <v>291.18</v>
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t>2 910 грн.</t>
+          <t>3 228 грн.</t>
         </is>
       </c>
     </row>
@@ -629,11 +629,11 @@
       </c>
       <c r="B28" s="0" t="inlineStr">
         <is>
-          <t>Rozetka.ua</t>
+          <t>Brain.com.ua</t>
         </is>
       </c>
       <c r="C28" s="0" t="n">
-        <v>269.16</v>
+        <v>270.52</v>
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
@@ -644,120 +644,120 @@
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B29" s="0" t="inlineStr">
         <is>
-          <t>TTN.by</t>
+          <t>Цифра</t>
         </is>
       </c>
       <c r="C29" s="0" t="n">
-        <v>302.6</v>
+        <v>262.5</v>
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>2 910 грн.</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B30" s="0" t="inlineStr">
         <is>
-          <t>SOCKET.BY</t>
+          <t>Епіцентр</t>
         </is>
       </c>
       <c r="C30" s="0" t="n">
-        <v>283.23</v>
+        <v>270.52</v>
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>2 999 грн.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B31" s="0" t="inlineStr">
         <is>
-          <t>Sli.by</t>
+          <t>Denika.ua</t>
         </is>
       </c>
       <c r="C31" s="0" t="n">
-        <v>283.23</v>
+        <v>270.52</v>
       </c>
       <c r="D31" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>2 999 грн.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B32" s="0" t="inlineStr">
         <is>
-          <t>RULEZ.BY</t>
+          <t>Stylus.ua</t>
         </is>
       </c>
       <c r="C32" s="0" t="n">
-        <v>302.07</v>
+        <v>271.52</v>
       </c>
       <c r="D32" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>3 010 грн.</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B33" s="0" t="inlineStr">
         <is>
-          <t>ITMarket.by</t>
+          <t>АЛЛО</t>
         </is>
       </c>
       <c r="C33" s="0" t="n">
-        <v>286.23</v>
+        <v>270.52</v>
       </c>
       <c r="D33" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>2 999 грн.</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B34" s="0" t="inlineStr">
         <is>
-          <t>imarket.by</t>
+          <t>Rozetka.ua</t>
         </is>
       </c>
       <c r="C34" s="0" t="n">
-        <v>340.51</v>
+        <v>270.52</v>
       </c>
       <c r="D34" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>2 999 грн.</t>
         </is>
       </c>
     </row>
@@ -769,11 +769,11 @@
       </c>
       <c r="B35" s="0" t="inlineStr">
         <is>
-          <t>AMD.by</t>
+          <t>SOCKET.BY</t>
         </is>
       </c>
       <c r="C35" s="0" t="n">
-        <v>289.14</v>
+        <v>283.23</v>
       </c>
       <c r="D35" s="0" t="inlineStr">
         <is>
@@ -789,11 +789,11 @@
       </c>
       <c r="B36" s="0" t="inlineStr">
         <is>
-          <t>VIPCOMP.BY</t>
+          <t>TTN.by</t>
         </is>
       </c>
       <c r="C36" s="0" t="n">
-        <v>302.07</v>
+        <v>302.6</v>
       </c>
       <c r="D36" s="0" t="inlineStr">
         <is>
@@ -809,11 +809,11 @@
       </c>
       <c r="B37" s="0" t="inlineStr">
         <is>
-          <t>24shop.by</t>
+          <t>KST.by</t>
         </is>
       </c>
       <c r="C37" s="0" t="n">
-        <v>307.25</v>
+        <v>283.23</v>
       </c>
       <c r="D37" s="0" t="inlineStr">
         <is>
@@ -829,11 +829,11 @@
       </c>
       <c r="B38" s="0" t="inlineStr">
         <is>
-          <t>itx.by</t>
+          <t>VIPCOMP.BY</t>
         </is>
       </c>
       <c r="C38" s="0" t="n">
-        <v>337.87</v>
+        <v>301.35</v>
       </c>
       <c r="D38" s="0" t="inlineStr">
         <is>
@@ -849,11 +849,11 @@
       </c>
       <c r="B39" s="0" t="inlineStr">
         <is>
-          <t>Медиа Маркет групп ООО</t>
+          <t>Sli.by</t>
         </is>
       </c>
       <c r="C39" s="0" t="n">
-        <v>308.93</v>
+        <v>283.23</v>
       </c>
       <c r="D39" s="0" t="inlineStr">
         <is>
@@ -873,7 +873,7 @@
         </is>
       </c>
       <c r="C40" s="0" t="n">
-        <v>307.25</v>
+        <v>302.07</v>
       </c>
       <c r="D40" s="0" t="inlineStr">
         <is>
@@ -909,11 +909,11 @@
       </c>
       <c r="B42" s="0" t="inlineStr">
         <is>
-          <t>bigi</t>
+          <t>Медиа Маркет групп ООО</t>
         </is>
       </c>
       <c r="C42" s="0" t="n">
-        <v>307.25</v>
+        <v>308.93</v>
       </c>
       <c r="D42" s="0" t="inlineStr">
         <is>
@@ -929,11 +929,11 @@
       </c>
       <c r="B43" s="0" t="inlineStr">
         <is>
-          <t>5 элемент</t>
+          <t>24shop.by</t>
         </is>
       </c>
       <c r="C43" s="0" t="n">
-        <v>359.0</v>
+        <v>307.25</v>
       </c>
       <c r="D43" s="0" t="inlineStr">
         <is>
@@ -949,11 +949,11 @@
       </c>
       <c r="B44" s="0" t="inlineStr">
         <is>
-          <t>ЭваЛайф</t>
+          <t>5 элемент</t>
         </is>
       </c>
       <c r="C44" s="0" t="n">
-        <v>283.23</v>
+        <v>359.0</v>
       </c>
       <c r="D44" s="0" t="inlineStr">
         <is>
@@ -969,11 +969,11 @@
       </c>
       <c r="B45" s="0" t="inlineStr">
         <is>
-          <t>KST.by</t>
+          <t>ViP MARKET</t>
         </is>
       </c>
       <c r="C45" s="0" t="n">
-        <v>283.23</v>
+        <v>323.29</v>
       </c>
       <c r="D45" s="0" t="inlineStr">
         <is>
@@ -989,11 +989,11 @@
       </c>
       <c r="B46" s="0" t="inlineStr">
         <is>
-          <t>21vek.by</t>
+          <t>ITMarket.by</t>
         </is>
       </c>
       <c r="C46" s="0" t="n">
-        <v>329.0</v>
+        <v>286.23</v>
       </c>
       <c r="D46" s="0" t="inlineStr">
         <is>
@@ -1009,11 +1009,11 @@
       </c>
       <c r="B47" s="0" t="inlineStr">
         <is>
-          <t>ЭЛЕКТРОСИЛА</t>
+          <t>bigi</t>
         </is>
       </c>
       <c r="C47" s="0" t="n">
-        <v>326.0</v>
+        <v>307.25</v>
       </c>
       <c r="D47" s="0" t="inlineStr">
         <is>
@@ -1029,11 +1029,11 @@
       </c>
       <c r="B48" s="0" t="inlineStr">
         <is>
-          <t>ViP MARKET</t>
+          <t>ЭЛЕКТРОСИЛА</t>
         </is>
       </c>
       <c r="C48" s="0" t="n">
-        <v>323.29</v>
+        <v>326.0</v>
       </c>
       <c r="D48" s="0" t="inlineStr">
         <is>
@@ -1049,13 +1049,233 @@
       </c>
       <c r="B49" s="0" t="inlineStr">
         <is>
+          <t>ЧУП "СВКомп"</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>320.0</v>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>RULEZ.BY</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>302.07</v>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>izliv.by</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>301.35</v>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B52" s="0" t="inlineStr">
+        <is>
+          <t>ВИКО-ТЕХНО</t>
+        </is>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>317.0</v>
+      </c>
+      <c r="D52" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B53" s="0" t="inlineStr">
+        <is>
+          <t>LevelUP</t>
+        </is>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>317.0</v>
+      </c>
+      <c r="D53" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B54" s="0" t="inlineStr">
+        <is>
+          <t>Itsmart.by</t>
+        </is>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>391.32</v>
+      </c>
+      <c r="D54" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B55" s="0" t="inlineStr">
+        <is>
+          <t>AMD.by</t>
+        </is>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>290.33</v>
+      </c>
+      <c r="D55" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B56" s="0" t="inlineStr">
+        <is>
+          <t>itx.by</t>
+        </is>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>337.87</v>
+      </c>
+      <c r="D56" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B57" s="0" t="inlineStr">
+        <is>
+          <t>BITS.By</t>
+        </is>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>317.0</v>
+      </c>
+      <c r="D57" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B58" s="0" t="inlineStr">
+        <is>
           <t>Мультиком.</t>
         </is>
       </c>
-      <c r="C49" s="0" t="n">
-        <v>308.18</v>
-      </c>
-      <c r="D49" s="0" t="inlineStr">
+      <c r="C58" s="0" t="n">
+        <v>310.08</v>
+      </c>
+      <c r="D58" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B59" s="0" t="inlineStr">
+        <is>
+          <t>21vek.by</t>
+        </is>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>329.0</v>
+      </c>
+      <c r="D59" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B60" s="0" t="inlineStr">
+        <is>
+          <t>imarket.by</t>
+        </is>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>340.51</v>
+      </c>
+      <c r="D60" s="0" t="inlineStr">
         <is>
           <t/>
         </is>

</xml_diff>

<commit_message>
refactor: split parts of parser
</commit_message>
<xml_diff>
--- a/prices.xlsx
+++ b/prices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <sheets>
-    <sheet sheetId="1" name="LG 24MK430H-B " r:id="rId4"/>
+    <sheet sheetId="1" name="LG 24GL600F-B " r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -67,7 +67,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -109,15 +109,15 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>E-first.ru</t>
+          <t>Официальный магазин LG</t>
         </is>
       </c>
       <c r="C2" s="0" t="n">
-        <v>325.59</v>
+        <v>491.56</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>9 535 р.</t>
+          <t>14 449 р.</t>
         </is>
       </c>
     </row>
@@ -129,15 +129,15 @@
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>Официальный магазин LG</t>
+          <t>Goods.ru</t>
         </is>
       </c>
       <c r="C3" s="0" t="n">
-        <v>324.36</v>
+        <v>523.57</v>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>9 499 р.</t>
+          <t>15 390 р.</t>
         </is>
       </c>
     </row>
@@ -149,15 +149,15 @@
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Goods.ru</t>
+          <t>Kns.ru</t>
         </is>
       </c>
       <c r="C4" s="0" t="n">
-        <v>305.27</v>
+        <v>546.78</v>
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>8 940 р.</t>
+          <t>16 072 р.</t>
         </is>
       </c>
     </row>
@@ -169,15 +169,15 @@
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>Kns.ru</t>
+          <t>Svyaznoy.ru</t>
         </is>
       </c>
       <c r="C5" s="0" t="n">
-        <v>298.65</v>
+        <v>575.28</v>
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>8 746 р.</t>
+          <t>16 910 р.</t>
         </is>
       </c>
     </row>
@@ -189,15 +189,15 @@
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>Svyaznoy.ru</t>
+          <t>CompYou.ru</t>
         </is>
       </c>
       <c r="C6" s="0" t="n">
-        <v>345.56</v>
+        <v>503.84</v>
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>10 120 р.</t>
+          <t>14 810 р.</t>
         </is>
       </c>
     </row>
@@ -209,15 +209,15 @@
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>Pleer.ru</t>
+          <t>Eldorado.ru</t>
         </is>
       </c>
       <c r="C7" s="0" t="n">
-        <v>286.12</v>
+        <v>523.57</v>
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>8 379 р.</t>
+          <t>15 390 р.</t>
         </is>
       </c>
     </row>
@@ -229,15 +229,15 @@
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>CompYou.ru</t>
+          <t>Elektro-park.ru</t>
         </is>
       </c>
       <c r="C8" s="0" t="n">
-        <v>298.27</v>
+        <v>522.55</v>
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>8 735 р.</t>
+          <t>15 360 р.</t>
         </is>
       </c>
     </row>
@@ -249,15 +249,15 @@
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>Eldorado.ru</t>
+          <t>Citilink.ru</t>
         </is>
       </c>
       <c r="C9" s="0" t="n">
-        <v>324.05</v>
+        <v>503.84</v>
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>9 490 р.</t>
+          <t>14 810 р.</t>
         </is>
       </c>
     </row>
@@ -269,15 +269,15 @@
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>Elektro-park.ru</t>
+          <t>123.ru</t>
         </is>
       </c>
       <c r="C10" s="0" t="n">
-        <v>305.95</v>
+        <v>533.1</v>
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>8 960 р.</t>
+          <t>15 670 р.</t>
         </is>
       </c>
     </row>
@@ -289,15 +289,15 @@
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>Citilink.ru</t>
+          <t>Империя Техно</t>
         </is>
       </c>
       <c r="C11" s="0" t="n">
-        <v>306.98</v>
+        <v>504.52</v>
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>8 990 р.</t>
+          <t>14 830 р.</t>
         </is>
       </c>
     </row>
@@ -309,15 +309,15 @@
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>Fotosklad.ru</t>
+          <t>М.видео</t>
         </is>
       </c>
       <c r="C12" s="0" t="n">
-        <v>317.22</v>
+        <v>523.57</v>
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t>9 290 р.</t>
+          <t>15 390 р.</t>
         </is>
       </c>
     </row>
@@ -329,15 +329,15 @@
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>ABC.ru</t>
+          <t>Pcplanet.ru</t>
         </is>
       </c>
       <c r="C13" s="0" t="n">
-        <v>316.92</v>
+        <v>557.63</v>
       </c>
       <c r="D13" s="0" t="inlineStr">
         <is>
-          <t>9 281 р.</t>
+          <t>16 391 р.</t>
         </is>
       </c>
     </row>
@@ -349,115 +349,115 @@
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>123.ru</t>
+          <t>Topcomputer.ru</t>
         </is>
       </c>
       <c r="C14" s="0" t="n">
-        <v>312.44</v>
+        <v>475.6</v>
       </c>
       <c r="D14" s="0" t="inlineStr">
         <is>
-          <t>9 150 р.</t>
+          <t>13 980 р.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>RUS</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>М.видео</t>
+          <t>Itbox.ua</t>
         </is>
       </c>
       <c r="C15" s="0" t="n">
-        <v>324.05</v>
+        <v>430.91</v>
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
-          <t>9 490 р.</t>
+          <t>4 777 грн.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>RUS</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>Just.ru</t>
+          <t>LuxPRO.ua</t>
         </is>
       </c>
       <c r="C16" s="0" t="n">
-        <v>310.39</v>
+        <v>430.91</v>
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
-          <t>9 090 р.</t>
+          <t>4 777 грн.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>RUS</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>Pcplanet.ru</t>
+          <t>Repka.ua</t>
         </is>
       </c>
       <c r="C17" s="0" t="n">
-        <v>334.3</v>
+        <v>431.27</v>
       </c>
       <c r="D17" s="0" t="inlineStr">
         <is>
-          <t>9 790 р.</t>
+          <t>4 781 грн.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>RUS</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>Kotofoto.ru</t>
+          <t>A-techno.com.ua</t>
         </is>
       </c>
       <c r="C18" s="0" t="n">
-        <v>337.03</v>
+        <v>430.91</v>
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
-          <t>9 870 р.</t>
+          <t>4 777 грн.</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>RUS</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>Topcomputer.ru</t>
+          <t>Homebt.com.ua</t>
         </is>
       </c>
       <c r="C19" s="0" t="n">
-        <v>285.81</v>
+        <v>451.03</v>
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
-          <t>8 370 р.</t>
+          <t>5 000 грн.</t>
         </is>
       </c>
     </row>
@@ -469,15 +469,15 @@
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>Itbox.ua</t>
+          <t>Isklad.tk</t>
         </is>
       </c>
       <c r="C20" s="0" t="n">
-        <v>270.52</v>
+        <v>430.91</v>
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
-          <t>2 999 грн.</t>
+          <t>4 777 грн.</t>
         </is>
       </c>
     </row>
@@ -489,15 +489,15 @@
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>LuxPRO.ua</t>
+          <t>Brain.com.ua</t>
         </is>
       </c>
       <c r="C21" s="0" t="n">
-        <v>270.52</v>
+        <v>430.91</v>
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
-          <t>2 999 грн.</t>
+          <t>4 777 грн.</t>
         </is>
       </c>
     </row>
@@ -509,15 +509,15 @@
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>V10.com.ua</t>
+          <t>Цифра</t>
         </is>
       </c>
       <c r="C22" s="0" t="n">
-        <v>393.02</v>
+        <v>425.41</v>
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t>4 357 грн.</t>
+          <t>4 716 грн.</t>
         </is>
       </c>
     </row>
@@ -529,15 +529,15 @@
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>Foroom.com.ua</t>
+          <t>FOXTROT.UA</t>
         </is>
       </c>
       <c r="C23" s="0" t="n">
-        <v>306.97</v>
+        <v>430.91</v>
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t>3 403 грн.</t>
+          <t>4 777 грн.</t>
         </is>
       </c>
     </row>
@@ -549,15 +549,15 @@
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>Repka.ua</t>
+          <t>Епіцентр</t>
         </is>
       </c>
       <c r="C24" s="0" t="n">
-        <v>267.46</v>
+        <v>430.91</v>
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t>2 965 грн.</t>
+          <t>4 777 грн.</t>
         </is>
       </c>
     </row>
@@ -569,15 +569,15 @@
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>A-techno.com.ua</t>
+          <t>Zhuk.ua</t>
         </is>
       </c>
       <c r="C25" s="0" t="n">
-        <v>270.52</v>
+        <v>430.91</v>
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
-          <t>2 999 грн.</t>
+          <t>4 777 грн.</t>
         </is>
       </c>
     </row>
@@ -589,15 +589,15 @@
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>Homebt.com.ua</t>
+          <t>Stylus.ua</t>
         </is>
       </c>
       <c r="C26" s="0" t="n">
-        <v>286.58</v>
+        <v>425.41</v>
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t>3 177 грн.</t>
+          <t>4 716 грн.</t>
         </is>
       </c>
     </row>
@@ -609,15 +609,15 @@
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>Hbox.com.ua</t>
+          <t>АЛЛО</t>
         </is>
       </c>
       <c r="C27" s="0" t="n">
-        <v>291.18</v>
+        <v>430.91</v>
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t>3 228 грн.</t>
+          <t>4 777 грн.</t>
         </is>
       </c>
     </row>
@@ -629,15 +629,15 @@
       </c>
       <c r="B28" s="0" t="inlineStr">
         <is>
-          <t>Brain.com.ua</t>
+          <t>Denika.ua</t>
         </is>
       </c>
       <c r="C28" s="0" t="n">
-        <v>270.52</v>
+        <v>430.91</v>
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
-          <t>2 999 грн.</t>
+          <t>4 777 грн.</t>
         </is>
       </c>
     </row>
@@ -649,15 +649,15 @@
       </c>
       <c r="B29" s="0" t="inlineStr">
         <is>
-          <t>Цифра</t>
+          <t>Palladium.ua</t>
         </is>
       </c>
       <c r="C29" s="0" t="n">
-        <v>262.5</v>
+        <v>430.91</v>
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
-          <t>2 910 грн.</t>
+          <t>4 777 грн.</t>
         </is>
       </c>
     </row>
@@ -669,15 +669,15 @@
       </c>
       <c r="B30" s="0" t="inlineStr">
         <is>
-          <t>Епіцентр</t>
+          <t>Hbox.com.ua</t>
         </is>
       </c>
       <c r="C30" s="0" t="n">
-        <v>270.52</v>
+        <v>466.09</v>
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
-          <t>2 999 грн.</t>
+          <t>5 167 грн.</t>
         </is>
       </c>
     </row>
@@ -689,75 +689,75 @@
       </c>
       <c r="B31" s="0" t="inlineStr">
         <is>
-          <t>Denika.ua</t>
+          <t>Rozetka.ua</t>
         </is>
       </c>
       <c r="C31" s="0" t="n">
-        <v>270.52</v>
+        <v>430.91</v>
       </c>
       <c r="D31" s="0" t="inlineStr">
         <is>
-          <t>2 999 грн.</t>
+          <t>4 777 грн.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>UA</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="B32" s="0" t="inlineStr">
         <is>
-          <t>Stylus.ua</t>
+          <t>SOCKET.BY</t>
         </is>
       </c>
       <c r="C32" s="0" t="n">
-        <v>271.52</v>
+        <v>555.0</v>
       </c>
       <c r="D32" s="0" t="inlineStr">
         <is>
-          <t>3 010 грн.</t>
+          <t/>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>UA</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="B33" s="0" t="inlineStr">
         <is>
-          <t>АЛЛО</t>
+          <t>TTN.by</t>
         </is>
       </c>
       <c r="C33" s="0" t="n">
-        <v>270.52</v>
+        <v>561.87</v>
       </c>
       <c r="D33" s="0" t="inlineStr">
         <is>
-          <t>2 999 грн.</t>
+          <t/>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>UA</t>
+          <t>BLR</t>
         </is>
       </c>
       <c r="B34" s="0" t="inlineStr">
         <is>
-          <t>Rozetka.ua</t>
+          <t>KST.by</t>
         </is>
       </c>
       <c r="C34" s="0" t="n">
-        <v>270.52</v>
+        <v>555.0</v>
       </c>
       <c r="D34" s="0" t="inlineStr">
         <is>
-          <t>2 999 грн.</t>
+          <t/>
         </is>
       </c>
     </row>
@@ -769,11 +769,11 @@
       </c>
       <c r="B35" s="0" t="inlineStr">
         <is>
-          <t>SOCKET.BY</t>
+          <t>VIPCOMP.BY</t>
         </is>
       </c>
       <c r="C35" s="0" t="n">
-        <v>283.23</v>
+        <v>555.0</v>
       </c>
       <c r="D35" s="0" t="inlineStr">
         <is>
@@ -789,11 +789,11 @@
       </c>
       <c r="B36" s="0" t="inlineStr">
         <is>
-          <t>TTN.by</t>
+          <t>Sli.by</t>
         </is>
       </c>
       <c r="C36" s="0" t="n">
-        <v>302.6</v>
+        <v>555.0</v>
       </c>
       <c r="D36" s="0" t="inlineStr">
         <is>
@@ -809,11 +809,11 @@
       </c>
       <c r="B37" s="0" t="inlineStr">
         <is>
-          <t>KST.by</t>
+          <t>Техник-Сервис</t>
         </is>
       </c>
       <c r="C37" s="0" t="n">
-        <v>283.23</v>
+        <v>576.42</v>
       </c>
       <c r="D37" s="0" t="inlineStr">
         <is>
@@ -829,11 +829,11 @@
       </c>
       <c r="B38" s="0" t="inlineStr">
         <is>
-          <t>VIPCOMP.BY</t>
+          <t>izliv.by</t>
         </is>
       </c>
       <c r="C38" s="0" t="n">
-        <v>301.35</v>
+        <v>555.0</v>
       </c>
       <c r="D38" s="0" t="inlineStr">
         <is>
@@ -849,11 +849,11 @@
       </c>
       <c r="B39" s="0" t="inlineStr">
         <is>
-          <t>Sli.by</t>
+          <t>Медиа Маркет групп ООО</t>
         </is>
       </c>
       <c r="C39" s="0" t="n">
-        <v>283.23</v>
+        <v>582.37</v>
       </c>
       <c r="D39" s="0" t="inlineStr">
         <is>
@@ -869,11 +869,11 @@
       </c>
       <c r="B40" s="0" t="inlineStr">
         <is>
-          <t>Техник-Сервис</t>
+          <t>ЧУП "СВКомп"</t>
         </is>
       </c>
       <c r="C40" s="0" t="n">
-        <v>302.07</v>
+        <v>610.0</v>
       </c>
       <c r="D40" s="0" t="inlineStr">
         <is>
@@ -889,11 +889,11 @@
       </c>
       <c r="B41" s="0" t="inlineStr">
         <is>
-          <t>Ньютон</t>
+          <t>ITMarket.by</t>
         </is>
       </c>
       <c r="C41" s="0" t="n">
-        <v>310.0</v>
+        <v>559.32</v>
       </c>
       <c r="D41" s="0" t="inlineStr">
         <is>
@@ -909,11 +909,11 @@
       </c>
       <c r="B42" s="0" t="inlineStr">
         <is>
-          <t>Медиа Маркет групп ООО</t>
+          <t>Ньютон</t>
         </is>
       </c>
       <c r="C42" s="0" t="n">
-        <v>308.93</v>
+        <v>555.0</v>
       </c>
       <c r="D42" s="0" t="inlineStr">
         <is>
@@ -929,11 +929,11 @@
       </c>
       <c r="B43" s="0" t="inlineStr">
         <is>
-          <t>24shop.by</t>
+          <t>Itsmart.by</t>
         </is>
       </c>
       <c r="C43" s="0" t="n">
-        <v>307.25</v>
+        <v>586.12</v>
       </c>
       <c r="D43" s="0" t="inlineStr">
         <is>
@@ -949,11 +949,11 @@
       </c>
       <c r="B44" s="0" t="inlineStr">
         <is>
-          <t>5 элемент</t>
+          <t>AMD.by</t>
         </is>
       </c>
       <c r="C44" s="0" t="n">
-        <v>359.0</v>
+        <v>576.42</v>
       </c>
       <c r="D44" s="0" t="inlineStr">
         <is>
@@ -969,11 +969,11 @@
       </c>
       <c r="B45" s="0" t="inlineStr">
         <is>
-          <t>ViP MARKET</t>
+          <t>imarket.by</t>
         </is>
       </c>
       <c r="C45" s="0" t="n">
-        <v>323.29</v>
+        <v>622.05</v>
       </c>
       <c r="D45" s="0" t="inlineStr">
         <is>
@@ -989,11 +989,11 @@
       </c>
       <c r="B46" s="0" t="inlineStr">
         <is>
-          <t>ITMarket.by</t>
+          <t>ЭЛЕКТРОСИЛА</t>
         </is>
       </c>
       <c r="C46" s="0" t="n">
-        <v>286.23</v>
+        <v>622.0</v>
       </c>
       <c r="D46" s="0" t="inlineStr">
         <is>
@@ -1009,11 +1009,11 @@
       </c>
       <c r="B47" s="0" t="inlineStr">
         <is>
-          <t>bigi</t>
+          <t>ViP MARKET</t>
         </is>
       </c>
       <c r="C47" s="0" t="n">
-        <v>307.25</v>
+        <v>606.39</v>
       </c>
       <c r="D47" s="0" t="inlineStr">
         <is>
@@ -1029,11 +1029,11 @@
       </c>
       <c r="B48" s="0" t="inlineStr">
         <is>
-          <t>ЭЛЕКТРОСИЛА</t>
+          <t>itx.by</t>
         </is>
       </c>
       <c r="C48" s="0" t="n">
-        <v>326.0</v>
+        <v>646.11</v>
       </c>
       <c r="D48" s="0" t="inlineStr">
         <is>
@@ -1049,11 +1049,11 @@
       </c>
       <c r="B49" s="0" t="inlineStr">
         <is>
-          <t>ЧУП "СВКомп"</t>
+          <t>BITS.By</t>
         </is>
       </c>
       <c r="C49" s="0" t="n">
-        <v>320.0</v>
+        <v>606.0</v>
       </c>
       <c r="D49" s="0" t="inlineStr">
         <is>
@@ -1069,11 +1069,11 @@
       </c>
       <c r="B50" s="0" t="inlineStr">
         <is>
-          <t>RULEZ.BY</t>
+          <t>ВИКО-ТЕХНО</t>
         </is>
       </c>
       <c r="C50" s="0" t="n">
-        <v>302.07</v>
+        <v>606.0</v>
       </c>
       <c r="D50" s="0" t="inlineStr">
         <is>
@@ -1089,11 +1089,11 @@
       </c>
       <c r="B51" s="0" t="inlineStr">
         <is>
-          <t>izliv.by</t>
+          <t>Мультиком.</t>
         </is>
       </c>
       <c r="C51" s="0" t="n">
-        <v>301.35</v>
+        <v>556.68</v>
       </c>
       <c r="D51" s="0" t="inlineStr">
         <is>
@@ -1109,11 +1109,11 @@
       </c>
       <c r="B52" s="0" t="inlineStr">
         <is>
-          <t>ВИКО-ТЕХНО</t>
+          <t>5 элемент</t>
         </is>
       </c>
       <c r="C52" s="0" t="n">
-        <v>317.0</v>
+        <v>699.0</v>
       </c>
       <c r="D52" s="0" t="inlineStr">
         <is>
@@ -1129,11 +1129,11 @@
       </c>
       <c r="B53" s="0" t="inlineStr">
         <is>
-          <t>LevelUP</t>
+          <t>bigi</t>
         </is>
       </c>
       <c r="C53" s="0" t="n">
-        <v>317.0</v>
+        <v>555.0</v>
       </c>
       <c r="D53" s="0" t="inlineStr">
         <is>
@@ -1149,11 +1149,11 @@
       </c>
       <c r="B54" s="0" t="inlineStr">
         <is>
-          <t>Itsmart.by</t>
+          <t>24shop.by</t>
         </is>
       </c>
       <c r="C54" s="0" t="n">
-        <v>391.32</v>
+        <v>555.0</v>
       </c>
       <c r="D54" s="0" t="inlineStr">
         <is>
@@ -1169,11 +1169,11 @@
       </c>
       <c r="B55" s="0" t="inlineStr">
         <is>
-          <t>AMD.by</t>
+          <t>21vek.by</t>
         </is>
       </c>
       <c r="C55" s="0" t="n">
-        <v>290.33</v>
+        <v>606.0</v>
       </c>
       <c r="D55" s="0" t="inlineStr">
         <is>
@@ -1189,93 +1189,13 @@
       </c>
       <c r="B56" s="0" t="inlineStr">
         <is>
-          <t>itx.by</t>
+          <t>LevelUP</t>
         </is>
       </c>
       <c r="C56" s="0" t="n">
-        <v>337.87</v>
+        <v>606.0</v>
       </c>
       <c r="D56" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="0" t="inlineStr">
-        <is>
-          <t>BLR</t>
-        </is>
-      </c>
-      <c r="B57" s="0" t="inlineStr">
-        <is>
-          <t>BITS.By</t>
-        </is>
-      </c>
-      <c r="C57" s="0" t="n">
-        <v>317.0</v>
-      </c>
-      <c r="D57" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="0" t="inlineStr">
-        <is>
-          <t>BLR</t>
-        </is>
-      </c>
-      <c r="B58" s="0" t="inlineStr">
-        <is>
-          <t>Мультиком.</t>
-        </is>
-      </c>
-      <c r="C58" s="0" t="n">
-        <v>310.08</v>
-      </c>
-      <c r="D58" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="0" t="inlineStr">
-        <is>
-          <t>BLR</t>
-        </is>
-      </c>
-      <c r="B59" s="0" t="inlineStr">
-        <is>
-          <t>21vek.by</t>
-        </is>
-      </c>
-      <c r="C59" s="0" t="n">
-        <v>329.0</v>
-      </c>
-      <c r="D59" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="0" t="inlineStr">
-        <is>
-          <t>BLR</t>
-        </is>
-      </c>
-      <c r="B60" s="0" t="inlineStr">
-        <is>
-          <t>imarket.by</t>
-        </is>
-      </c>
-      <c r="C60" s="0" t="n">
-        <v>340.51</v>
-      </c>
-      <c r="D60" s="0" t="inlineStr">
         <is>
           <t/>
         </is>

</xml_diff>

<commit_message>
fix: when shown color of good - parse price
</commit_message>
<xml_diff>
--- a/prices.xlsx
+++ b/prices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <sheets>
-    <sheet sheetId="1" name="Samsung Galaxy A51 " r:id="rId4"/>
+    <sheet sheetId="1" name="Galaxy S20 Ultra " r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -67,7 +67,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -76,7 +76,7 @@
     <col min="1" max="1" bestFit="1" customWidth="1" width="8.8"/>
     <col min="2" max="2" bestFit="1" customWidth="1" width="31.900000000000002"/>
     <col min="3" max="3" bestFit="1" customWidth="1" width="11.0"/>
-    <col min="4" max="4" bestFit="1" customWidth="1" width="7.700000000000001"/>
+    <col min="4" max="4" bestFit="1" customWidth="1" width="14.3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -104,598 +104,1378 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Мобилайн</t>
+          <t>Appleavenue.ru</t>
         </is>
       </c>
       <c r="C2" s="0" t="n">
-        <v>726.0</v>
+        <v>2659.25</v>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>77 550 р.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>ТЕХНОСИЛА</t>
+          <t>Video-shoper.ru</t>
         </is>
       </c>
       <c r="C3" s="0" t="n">
-        <v>726.0</v>
+        <v>2509.74</v>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>73 190 р.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>МОБИСТАР</t>
+          <t>Gsm10.ru</t>
         </is>
       </c>
       <c r="C4" s="0" t="n">
-        <v>726.0</v>
+        <v>2431.22</v>
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>70 900 р.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>7 дней</t>
+          <t>ДжастокРу</t>
         </is>
       </c>
       <c r="C5" s="0" t="n">
-        <v>670.0</v>
+        <v>2417.12</v>
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>70 489 р.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>ТЕХНОМИР</t>
+          <t>Formulatv.ru</t>
         </is>
       </c>
       <c r="C6" s="0" t="n">
-        <v>0.0</v>
+        <v>2742.92</v>
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>79 990 р.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>"Техно"</t>
+          <t>Goods.ru</t>
         </is>
       </c>
       <c r="C7" s="0" t="n">
-        <v>670.0</v>
+        <v>3771.65</v>
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>109 990 р.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>Zvonok</t>
+          <t>Cifrus.ru</t>
         </is>
       </c>
       <c r="C8" s="0" t="n">
-        <v>0.0</v>
+        <v>2451.45</v>
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>71 490 р.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>ТеХнИкС</t>
+          <t>Galaxystore.ru</t>
         </is>
       </c>
       <c r="C9" s="0" t="n">
-        <v>670.0</v>
+        <v>2914.38</v>
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>84 990 р.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>AMD.by</t>
+          <t>Svyaznoy.ru</t>
         </is>
       </c>
       <c r="C10" s="0" t="n">
-        <v>727.0</v>
+        <v>2914.38</v>
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>84 990 р.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>АЛЛОплюс</t>
+          <t>Holodilnik.ru</t>
         </is>
       </c>
       <c r="C11" s="0" t="n">
-        <v>754.55</v>
+        <v>3325.87</v>
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>96 990 р.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>Телефоника</t>
+          <t>Ogo1.ru</t>
         </is>
       </c>
       <c r="C12" s="0" t="n">
-        <v>863.34</v>
+        <v>3082.74</v>
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>89 900 р.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>Мегастор</t>
+          <t>Xcom-shop.ru</t>
         </is>
       </c>
       <c r="C13" s="0" t="n">
-        <v>799.0</v>
+        <v>3427.37</v>
       </c>
       <c r="D13" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>99 950 р.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>OnlineGSM</t>
+          <t>KomfortBT.ru</t>
         </is>
       </c>
       <c r="C14" s="0" t="n">
-        <v>728.0</v>
+        <v>3279.23</v>
       </c>
       <c r="D14" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>95 630 р.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>24shop.by</t>
+          <t>Eldorado.ru</t>
         </is>
       </c>
       <c r="C15" s="0" t="n">
-        <v>670.0</v>
+        <v>3428.74</v>
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>99 990 р.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>Agroup.by</t>
+          <t>Moviand.ru</t>
         </is>
       </c>
       <c r="C16" s="0" t="n">
-        <v>725.0</v>
+        <v>2503.23</v>
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>73 000 р.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>bigi</t>
+          <t>Megafon.ru</t>
         </is>
       </c>
       <c r="C17" s="0" t="n">
-        <v>698.85</v>
+        <v>3428.74</v>
       </c>
       <c r="D17" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>99 990 р.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>MobilePlus</t>
+          <t>Flash Computers</t>
         </is>
       </c>
       <c r="C18" s="0" t="n">
-        <v>737.0</v>
+        <v>2450.42</v>
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>71 460 р.</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>imarket.by</t>
+          <t>Oldi.ru</t>
         </is>
       </c>
       <c r="C19" s="0" t="n">
-        <v>698.85</v>
+        <v>3600.19</v>
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>104 990 р.</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>forward</t>
+          <t>1click.ru</t>
         </is>
       </c>
       <c r="C20" s="0" t="n">
-        <v>739.0</v>
+        <v>3771.65</v>
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>109 990 р.</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>RUS</t>
         </is>
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>Унитарное предприятие "А1"</t>
+          <t>Gsmking.ru</t>
         </is>
       </c>
       <c r="C21" s="0" t="n">
-        <v>899.0</v>
+        <v>2606.07</v>
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>75 999 р.</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>JUST-MOBILE</t>
+          <t>Repka.ua</t>
         </is>
       </c>
       <c r="C22" s="0" t="n">
-        <v>670.0</v>
+        <v>3438.1</v>
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>37 999 грн.</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>21vek.by</t>
+          <t>Samsung Experience Store</t>
         </is>
       </c>
       <c r="C23" s="0" t="n">
-        <v>839.0</v>
+        <v>3980.98</v>
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>43 999 грн.</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>Ньютон</t>
+          <t>АЛЛО</t>
         </is>
       </c>
       <c r="C24" s="0" t="n">
-        <v>726.0</v>
+        <v>3438.1</v>
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>37 999 грн.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>Мобильный express</t>
+          <t>Fotomost.com.ua</t>
         </is>
       </c>
       <c r="C25" s="0" t="n">
-        <v>839.0</v>
+        <v>2579.91</v>
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>28 514 грн.</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>TTN.by</t>
+          <t>Easybay.com.ua</t>
         </is>
       </c>
       <c r="C26" s="0" t="n">
-        <v>790.15</v>
+        <v>2556.03</v>
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>28 250 грн.</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>Смарт Точка</t>
+          <t>Vodafone.ua</t>
         </is>
       </c>
       <c r="C27" s="0" t="n">
-        <v>670.0</v>
+        <v>3438.1</v>
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>37 999 грн.</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B28" s="0" t="inlineStr">
         <is>
-          <t>НА СВЯЗИ</t>
+          <t>Easymac.com.ua</t>
         </is>
       </c>
       <c r="C28" s="0" t="n">
-        <v>878.78</v>
+        <v>2821.13</v>
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>31 180 грн.</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>BLR</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="B29" s="0" t="inlineStr">
         <is>
-          <t>"ЕВРОСЕТЬ"</t>
+          <t>Ringoo.ua</t>
         </is>
       </c>
       <c r="C29" s="0" t="n">
-        <v>670.0</v>
+        <v>3438.1</v>
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>37 999 грн.</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>UA</t>
         </is>
       </c>
       <c r="B30" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>Brain.com.ua</t>
         </is>
       </c>
       <c r="C30" s="0" t="n">
-        <v>799.0</v>
+        <v>3438.1</v>
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>37 999 грн.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>UA</t>
         </is>
       </c>
       <c r="B31" s="0" t="inlineStr">
         <is>
-          <t/>
+          <t>COMFY.ua</t>
         </is>
       </c>
       <c r="C31" s="0" t="n">
-        <v>839.0</v>
+        <v>3438.1</v>
       </c>
       <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>37 999 грн.</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="inlineStr">
+        <is>
+          <t>UA</t>
+        </is>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>FOXTROT.UA</t>
+        </is>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>3438.1</v>
+      </c>
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>37 999 грн.</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="inlineStr">
+        <is>
+          <t>UA</t>
+        </is>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>AVR-group.com.ua</t>
+        </is>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>3147.76</v>
+      </c>
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>34 790 грн.</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="inlineStr">
+        <is>
+          <t>UA</t>
+        </is>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>Itbox.ua</t>
+        </is>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>3980.98</v>
+      </c>
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>43 999 грн.</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="inlineStr">
+        <is>
+          <t>UA</t>
+        </is>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>Zhuk.ua</t>
+        </is>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>3438.1</v>
+      </c>
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>37 999 грн.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="inlineStr">
+        <is>
+          <t>UA</t>
+        </is>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>Touchstudio.com.ua</t>
+        </is>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>2582.72</v>
+      </c>
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>28 545 грн.</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="inlineStr">
+        <is>
+          <t>UA</t>
+        </is>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>Cactus</t>
+        </is>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>3175.72</v>
+      </c>
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>35 099 грн.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="inlineStr">
+        <is>
+          <t>UA</t>
+        </is>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>Stylus.ua</t>
+        </is>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>3257.15</v>
+      </c>
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t>35 999 грн.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="inlineStr">
+        <is>
+          <t>UA</t>
+        </is>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>iTMag.ua</t>
+        </is>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>3438.1</v>
+      </c>
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>37 999 грн.</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="inlineStr">
+        <is>
+          <t>UA</t>
+        </is>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>Nofelet.ua</t>
+        </is>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>2641.89</v>
+      </c>
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>29 199 грн.</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="inlineStr">
+        <is>
+          <t>UA</t>
+        </is>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>Tehnopostavka.com.ua</t>
+        </is>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>2518.02</v>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>27 830 грн.</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>Мобилайн</t>
+        </is>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>2599.0</v>
+      </c>
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>ТЕХНОСИЛА</t>
+        </is>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>2599.0</v>
+      </c>
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>МОБИСТАР</t>
+        </is>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>2599.0</v>
+      </c>
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>7 дней</t>
+        </is>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>2599.0</v>
+      </c>
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>ТЕХНОМИР</t>
+        </is>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>2599.0</v>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>"Техно"</t>
+        </is>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>2599.0</v>
+      </c>
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>Zvonok</t>
+        </is>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>2599.0</v>
+      </c>
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>bigi</t>
+        </is>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>3075.57</v>
+      </c>
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>JUST-MOBILE</t>
+        </is>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>2599.0</v>
+      </c>
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>OnlineGSM</t>
+        </is>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>2599.0</v>
+      </c>
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B52" s="0" t="inlineStr">
+        <is>
+          <t>MobilePlus</t>
+        </is>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>2599.0</v>
+      </c>
+      <c r="D52" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B53" s="0" t="inlineStr">
+        <is>
+          <t>5 элемент</t>
+        </is>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>3499.0</v>
+      </c>
+      <c r="D53" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B54" s="0" t="inlineStr">
+        <is>
+          <t>AMD.by</t>
+        </is>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>2675.45</v>
+      </c>
+      <c r="D54" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B55" s="0" t="inlineStr">
+        <is>
+          <t>Смарт Точка</t>
+        </is>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>2599.0</v>
+      </c>
+      <c r="D55" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B56" s="0" t="inlineStr">
+        <is>
+          <t>Унитарное предприятие "А1"</t>
+        </is>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>3499.0</v>
+      </c>
+      <c r="D56" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B57" s="0" t="inlineStr">
+        <is>
+          <t>21vek.by</t>
+        </is>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>3499.0</v>
+      </c>
+      <c r="D57" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B58" s="0" t="inlineStr">
+        <is>
+          <t>Agroup.by</t>
+        </is>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>2599.0</v>
+      </c>
+      <c r="D58" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B59" s="0" t="inlineStr">
+        <is>
+          <t>imarket.by</t>
+        </is>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>3699.0</v>
+      </c>
+      <c r="D59" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B60" s="0" t="inlineStr">
+        <is>
+          <t>НА СВЯЗИ</t>
+        </is>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>3499.0</v>
+      </c>
+      <c r="D60" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B61" s="0" t="inlineStr">
+        <is>
+          <t>TTN.by</t>
+        </is>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>2854.95</v>
+      </c>
+      <c r="D61" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B62" s="0" t="inlineStr">
+        <is>
+          <t>Интернет-магазин МТС</t>
+        </is>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>3499.0</v>
+      </c>
+      <c r="D62" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B63" s="0" t="inlineStr">
+        <is>
+          <t>Мобильный express</t>
+        </is>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>2599.0</v>
+      </c>
+      <c r="D63" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B64" s="0" t="inlineStr">
+        <is>
+          <t>ЭваЛайф</t>
+        </is>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>3075.57</v>
+      </c>
+      <c r="D64" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B65" s="0" t="inlineStr">
+        <is>
+          <t>SOCKET.BY</t>
+        </is>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>2599.0</v>
+      </c>
+      <c r="D65" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B66" s="0" t="inlineStr">
+        <is>
+          <t>Мультиком.</t>
+        </is>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>3205.65</v>
+      </c>
+      <c r="D66" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B67" s="0" t="inlineStr">
+        <is>
+          <t>Ньютон</t>
+        </is>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>2599.0</v>
+      </c>
+      <c r="D67" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B68" s="0" t="inlineStr">
+        <is>
+          <t>forward</t>
+        </is>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>2599.0</v>
+      </c>
+      <c r="D68" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B69" s="0" t="inlineStr">
+        <is>
+          <t>24shop.by</t>
+        </is>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>3075.57</v>
+      </c>
+      <c r="D69" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="0" t="inlineStr">
+        <is>
+          <t>BLR</t>
+        </is>
+      </c>
+      <c r="B70" s="0" t="inlineStr">
+        <is>
+          <t>"ЕВРОСЕТЬ"</t>
+        </is>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>3599.0</v>
+      </c>
+      <c r="D70" s="0" t="inlineStr">
         <is>
           <t/>
         </is>

</xml_diff>